<commit_message>
save before NAACL submission
</commit_message>
<xml_diff>
--- a/justifs/mtir-lignos-etal-2019/MTIR-correlations.xlsx
+++ b/justifs/mtir-lignos-etal-2019/MTIR-correlations.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tg/work/papers/007-mt-eval-macro/justifs/mtir-lignos-etal-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8C0D7384-F1A3-824C-9127-2CA439E3D395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5A7209-78E8-9241-9631-013D23B81F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="60" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="380" yWindow="60" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MTIR-kendall" sheetId="1" r:id="rId1"/>
-    <sheet name="MTIR-pearson" sheetId="3" r:id="rId2"/>
+    <sheet name="MTIR-kendall-min" sheetId="4" r:id="rId1"/>
+    <sheet name="MTIR-kendall" sheetId="1" r:id="rId2"/>
+    <sheet name="MTIR-pearson" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="MTIR_pearson" localSheetId="1">'MTIR-pearson'!$A$1:$H$36</definedName>
+    <definedName name="MTIR_pearson" localSheetId="2">'MTIR-pearson'!$A$1:$H$36</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="MTIR-pearson" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/tg/work/papers/007-mt-eval-macro/justifs/mtir-lignos-etal-2019/MTIR-pearson.csv">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="MTIR-pearson" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/tg/work/papers/007-mt-eval-macro/justifs/mtir-lignos-etal-2019/MTIR-pearson.csv">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="19">
   <si>
     <t>Group</t>
   </si>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -599,11 +600,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -612,6 +610,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -695,7 +699,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MTIR-pearson" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MTIR-pearson" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -994,42 +998,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85121B43-5BBD-5846-8E0F-B08474BDE1CC}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1062,719 +1067,287 @@
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>0.81200000000000006</v>
+        <v>0.85</v>
       </c>
       <c r="D3">
-        <v>0.79500000000000004</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="E3">
-        <v>0.81200000000000006</v>
+        <v>0.85</v>
       </c>
       <c r="F3">
-        <v>0.81200000000000006</v>
+        <v>0.85</v>
       </c>
       <c r="G3">
-        <v>0.76200000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="H3">
-        <v>0.79500000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>0.65</v>
-      </c>
-      <c r="D4">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="E4">
-        <v>0.65</v>
-      </c>
-      <c r="F4">
-        <v>0.65</v>
-      </c>
-      <c r="G4">
-        <v>0.6</v>
-      </c>
-      <c r="H4">
-        <v>0.63300000000000001</v>
+        <v>0.86699999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>0.85</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="D5">
-        <v>0.86699999999999999</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="E5">
-        <v>0.85</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="F5">
-        <v>0.85</v>
+        <v>0.874</v>
       </c>
       <c r="G5">
-        <v>0.9</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="H5">
-        <v>0.86699999999999999</v>
+        <v>0.89500000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="D6">
-        <v>0.93300000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="E6">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="F6">
-        <v>0.95</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="G6">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="H6">
         <v>0.9</v>
       </c>
-      <c r="H6">
-        <v>0.93300000000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8">
-        <v>0.86199999999999999</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="D8">
-        <v>0.89500000000000002</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="E8">
-        <v>0.86199999999999999</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="F8">
-        <v>0.874</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="G8">
-        <v>0.91200000000000003</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="H8">
-        <v>0.89500000000000002</v>
+        <v>0.66700000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>0.79500000000000004</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="D9">
-        <v>0.79500000000000004</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="E9">
-        <v>0.79500000000000004</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="F9">
-        <v>0.80700000000000005</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="G9">
-        <v>0.81200000000000006</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="H9">
-        <v>0.79500000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>0.8</v>
-      </c>
-      <c r="D10">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="E10">
-        <v>0.8</v>
-      </c>
-      <c r="F10">
-        <v>0.81200000000000006</v>
-      </c>
-      <c r="G10">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="H10">
-        <v>0.8</v>
+        <v>0.66700000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="D11">
-        <v>0.9</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="E11">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="F11">
-        <v>0.91200000000000003</v>
+        <v>0.745</v>
       </c>
       <c r="G11">
-        <v>0.91700000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="H11">
-        <v>0.9</v>
+        <v>0.71699999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
-        <v>0.88300000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="D12">
-        <v>0.91700000000000004</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="E12">
-        <v>0.88300000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="F12">
-        <v>0.89500000000000002</v>
+        <v>0.745</v>
       </c>
       <c r="G12">
-        <v>0.93300000000000005</v>
+        <v>0.7</v>
       </c>
       <c r="H12">
-        <v>0.91700000000000004</v>
+        <v>0.71699999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>0.68300000000000005</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="D14">
-        <v>0.66700000000000004</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="E14">
-        <v>0.68300000000000005</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="F14">
-        <v>0.68300000000000005</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="G14">
-        <v>0.63300000000000001</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="H14">
-        <v>0.66700000000000004</v>
+        <v>0.61699999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>0.75600000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="D15">
-        <v>0.74</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="E15">
-        <v>0.75600000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="F15">
-        <v>0.75600000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="G15">
-        <v>0.70599999999999996</v>
+        <v>0.75</v>
       </c>
       <c r="H15">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="D16">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="E16">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="F16">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="G16">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="H16">
-        <v>0.71699999999999997</v>
+        <v>0.78300000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>0.68300000000000005</v>
+        <v>0.7</v>
       </c>
       <c r="D17">
         <v>0.66700000000000004</v>
       </c>
       <c r="E17">
+        <v>0.7</v>
+      </c>
+      <c r="F17">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="G17">
         <v>0.68300000000000005</v>
       </c>
-      <c r="F17">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="G17">
-        <v>0.63300000000000001</v>
-      </c>
       <c r="H17">
-        <v>0.66700000000000004</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="D18">
         <v>0.7</v>
       </c>
-      <c r="D18">
-        <v>0.68300000000000005</v>
-      </c>
       <c r="E18">
-        <v>0.7</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="F18">
-        <v>0.7</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="G18">
-        <v>0.65</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="H18">
-        <v>0.68300000000000005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20">
-        <v>0.75</v>
-      </c>
-      <c r="D20">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="E20">
-        <v>0.75</v>
-      </c>
-      <c r="F20">
-        <v>0.745</v>
-      </c>
-      <c r="G20">
-        <v>0.7</v>
-      </c>
-      <c r="H20">
-        <v>0.71699999999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="D21">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="E21">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="F21">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="G21">
-        <v>0.71099999999999997</v>
-      </c>
-      <c r="H21">
-        <v>0.72799999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22">
-        <v>0.75</v>
-      </c>
-      <c r="D22">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="E22">
-        <v>0.75</v>
-      </c>
-      <c r="F22">
-        <v>0.745</v>
-      </c>
-      <c r="G22">
-        <v>0.7</v>
-      </c>
-      <c r="H22">
-        <v>0.71699999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23">
-        <v>0.75</v>
-      </c>
-      <c r="D23">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="E23">
-        <v>0.75</v>
-      </c>
-      <c r="F23">
-        <v>0.745</v>
-      </c>
-      <c r="G23">
-        <v>0.7</v>
-      </c>
-      <c r="H23">
-        <v>0.71699999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24">
-        <v>0.75</v>
-      </c>
-      <c r="D24">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="E24">
-        <v>0.75</v>
-      </c>
-      <c r="F24">
-        <v>0.745</v>
-      </c>
-      <c r="G24">
-        <v>0.7</v>
-      </c>
-      <c r="H24">
-        <v>0.71699999999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="D26">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="E26">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="F26">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="G26">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="H26">
-        <v>0.61699999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="D27">
-        <v>0.7</v>
-      </c>
-      <c r="E27">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="F27">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="G27">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="H27">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="D28">
-        <v>0.7</v>
-      </c>
-      <c r="E28">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="F28">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="G28">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="H28">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29">
-        <v>0.8</v>
-      </c>
-      <c r="D29">
-        <v>0.78300000000000003</v>
-      </c>
-      <c r="E29">
-        <v>0.8</v>
-      </c>
-      <c r="F29">
-        <v>0.8</v>
-      </c>
-      <c r="G29">
-        <v>0.75</v>
-      </c>
-      <c r="H29">
-        <v>0.78300000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="D30">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="E30">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="F30">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="G30">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="H30">
-        <v>0.66700000000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32">
-        <v>0.7</v>
-      </c>
-      <c r="D32">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="E32">
-        <v>0.7</v>
-      </c>
-      <c r="F32">
-        <v>0.71099999999999997</v>
-      </c>
-      <c r="G32">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="H32">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="D33">
-        <v>0.59899999999999998</v>
-      </c>
-      <c r="E33">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="F33">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="G33">
-        <v>0.61599999999999999</v>
-      </c>
-      <c r="H33">
-        <v>0.63300000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="D34">
-        <v>0.6</v>
-      </c>
-      <c r="E34">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="F34">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="G34">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="H34">
-        <v>0.63300000000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="D35">
-        <v>0.7</v>
-      </c>
-      <c r="E35">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="F35">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="G35">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="H35">
         <v>0.73299999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="D36">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="E36">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="F36">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="G36">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="H36">
-        <v>0.65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A17:A18"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:H6 C32:H36 C26:H30 C20:H24 C8:H12 C14:H18">
+  <conditionalFormatting sqref="C2:H3 C5:H6 C8:H9 C11:H12 C14:H15 C17:H18">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>C2=MAX($C2:$H2)</formula>
     </cfRule>
@@ -1784,7 +1357,797 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>0.95</v>
+      </c>
+      <c r="D2">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="E2">
+        <v>0.95</v>
+      </c>
+      <c r="F2">
+        <v>0.95</v>
+      </c>
+      <c r="G2">
+        <v>0.9</v>
+      </c>
+      <c r="H2">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="D3">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E3">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="F3">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="G3">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.79500000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>0.65</v>
+      </c>
+      <c r="D4">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.65</v>
+      </c>
+      <c r="F4">
+        <v>0.65</v>
+      </c>
+      <c r="G4">
+        <v>0.6</v>
+      </c>
+      <c r="H4">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>0.85</v>
+      </c>
+      <c r="D5">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.85</v>
+      </c>
+      <c r="F5">
+        <v>0.85</v>
+      </c>
+      <c r="G5">
+        <v>0.9</v>
+      </c>
+      <c r="H5">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0.95</v>
+      </c>
+      <c r="D6">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="E6">
+        <v>0.95</v>
+      </c>
+      <c r="F6">
+        <v>0.95</v>
+      </c>
+      <c r="G6">
+        <v>0.9</v>
+      </c>
+      <c r="H6">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E8">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="F8">
+        <v>0.874</v>
+      </c>
+      <c r="G8">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="H8">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="D9">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E9">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F9">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="G9">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="H9">
+        <v>0.79500000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>0.8</v>
+      </c>
+      <c r="D10">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="E10">
+        <v>0.8</v>
+      </c>
+      <c r="F10">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="G10">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="H10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>0.9</v>
+      </c>
+      <c r="D11">
+        <v>0.9</v>
+      </c>
+      <c r="E11">
+        <v>0.9</v>
+      </c>
+      <c r="F11">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="G11">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="H11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="E12">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="G12">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="H12">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="D14">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="E14">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="F14">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="G14">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H14">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="D15">
+        <v>0.74</v>
+      </c>
+      <c r="E15">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="F15">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="G15">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="H15">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="D16">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E16">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="F16">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="G16">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="H16">
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="D17">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="E17">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="F17">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="G17">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H17">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>0.7</v>
+      </c>
+      <c r="D18">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="E18">
+        <v>0.7</v>
+      </c>
+      <c r="F18">
+        <v>0.7</v>
+      </c>
+      <c r="G18">
+        <v>0.65</v>
+      </c>
+      <c r="H18">
+        <v>0.68300000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>0.75</v>
+      </c>
+      <c r="D20">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E20">
+        <v>0.75</v>
+      </c>
+      <c r="F20">
+        <v>0.745</v>
+      </c>
+      <c r="G20">
+        <v>0.7</v>
+      </c>
+      <c r="H20">
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D21">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="E21">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="F21">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="G21">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="H21">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>0.75</v>
+      </c>
+      <c r="D22">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E22">
+        <v>0.75</v>
+      </c>
+      <c r="F22">
+        <v>0.745</v>
+      </c>
+      <c r="G22">
+        <v>0.7</v>
+      </c>
+      <c r="H22">
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>0.75</v>
+      </c>
+      <c r="D23">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E23">
+        <v>0.75</v>
+      </c>
+      <c r="F23">
+        <v>0.745</v>
+      </c>
+      <c r="G23">
+        <v>0.7</v>
+      </c>
+      <c r="H23">
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>0.75</v>
+      </c>
+      <c r="D24">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E24">
+        <v>0.75</v>
+      </c>
+      <c r="F24">
+        <v>0.745</v>
+      </c>
+      <c r="G24">
+        <v>0.7</v>
+      </c>
+      <c r="H24">
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="D26">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="E26">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="F26">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="H26">
+        <v>0.61699999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="D27">
+        <v>0.7</v>
+      </c>
+      <c r="E27">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="F27">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="G27">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="H27">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="D28">
+        <v>0.7</v>
+      </c>
+      <c r="E28">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="F28">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="G28">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="H28">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>0.8</v>
+      </c>
+      <c r="D29">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="E29">
+        <v>0.8</v>
+      </c>
+      <c r="F29">
+        <v>0.8</v>
+      </c>
+      <c r="G29">
+        <v>0.75</v>
+      </c>
+      <c r="H29">
+        <v>0.78300000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="D30">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="E30">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="F30">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="G30">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H30">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>0.7</v>
+      </c>
+      <c r="D32">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="E32">
+        <v>0.7</v>
+      </c>
+      <c r="F32">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="G32">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="H32">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D33">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="E33">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F33">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="G33">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="H33">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D34">
+        <v>0.6</v>
+      </c>
+      <c r="E34">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F34">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="G34">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="H34">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="D35">
+        <v>0.7</v>
+      </c>
+      <c r="E35">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="F35">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="G35">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="H35">
+        <v>0.73299999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="D36">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="E36">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="F36">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="G36">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H36">
+        <v>0.65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A26:A30"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:H6 C32:H36 C26:H30 C20:H24 C8:H12 C14:H18">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>C2=MAX($C2:$H2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -1803,34 +2166,34 @@
     <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -1856,7 +2219,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="6"/>
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1880,7 +2243,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1904,7 +2267,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1928,7 +2291,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -1952,7 +2315,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
@@ -1978,7 +2341,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2365,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -2026,7 +2389,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="6"/>
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -2050,7 +2413,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="6"/>
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -2074,7 +2437,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
@@ -2100,7 +2463,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -2124,7 +2487,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>11</v>
       </c>
@@ -2148,7 +2511,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="6"/>
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -2172,7 +2535,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="6"/>
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -2196,7 +2559,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
@@ -2222,7 +2585,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="6"/>
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -2246,7 +2609,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
+      <c r="A22" s="6"/>
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -2270,7 +2633,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="6"/>
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -2294,7 +2657,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
+      <c r="A24" s="6"/>
       <c r="B24" t="s">
         <v>13</v>
       </c>
@@ -2318,7 +2681,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
@@ -2344,7 +2707,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
+      <c r="A27" s="6"/>
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -2368,7 +2731,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
+      <c r="A28" s="6"/>
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -2392,7 +2755,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
+      <c r="A29" s="6"/>
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -2416,7 +2779,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
+      <c r="A30" s="6"/>
       <c r="B30" t="s">
         <v>13</v>
       </c>
@@ -2440,7 +2803,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B32" t="s">
@@ -2466,7 +2829,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+      <c r="A33" s="6"/>
       <c r="B33" t="s">
         <v>10</v>
       </c>
@@ -2490,7 +2853,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="6"/>
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -2514,7 +2877,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
+      <c r="A35" s="6"/>
       <c r="B35" t="s">
         <v>12</v>
       </c>
@@ -2538,7 +2901,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
+      <c r="A36" s="6"/>
       <c r="B36" t="s">
         <v>13</v>
       </c>
@@ -2563,15 +2926,15 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A32:A36"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A32:A36"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:H6 C32:H36 C26:H30 C20:H24 C14:H18 C8:H12">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>C2=MAX($C2:$H2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>